<commit_message>
modification pour le rendu du grep
</commit_message>
<xml_diff>
--- a/Dossier/Acceptation A2/Product backlog.xlsx
+++ b/Dossier/Acceptation A2/Product backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="588"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -173,6 +173,21 @@
   </si>
   <si>
     <t>Faire la base de données (créer la table)</t>
+  </si>
+  <si>
+    <t>En tant qu’utilisateur, je veux afficher les lignes Noctambus</t>
+  </si>
+  <si>
+    <t>En tant qu’utilisateur, je veux afficher les arrets d'une ligne</t>
+  </si>
+  <si>
+    <t>En tant qu’utilisateur, je veux afficher les départs prévus</t>
+  </si>
+  <si>
+    <t>STATUS Android</t>
+  </si>
+  <si>
+    <t>STATUS IOS</t>
   </si>
 </sst>
 </file>
@@ -375,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -395,7 +410,6 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -729,7 +743,7 @@
   <dimension ref="B1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,11 +753,12 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -760,10 +775,13 @@
         <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -780,10 +798,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -800,10 +821,13 @@
         <v>2</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>4</v>
       </c>
@@ -822,8 +846,11 @@
       <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>11</v>
       </c>
@@ -840,10 +867,13 @@
         <v>4</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -862,8 +892,11 @@
       <c r="G7" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>7</v>
       </c>
@@ -882,8 +915,11 @@
       <c r="G8" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
         <v>8</v>
       </c>
@@ -902,8 +938,11 @@
       <c r="G9" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>12</v>
       </c>
@@ -922,8 +961,11 @@
       <c r="G10" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>13</v>
       </c>
@@ -942,8 +984,11 @@
       <c r="G11" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <v>14</v>
       </c>
@@ -962,8 +1007,11 @@
       <c r="G12" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <v>15</v>
       </c>
@@ -982,8 +1030,11 @@
       <c r="G13" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <v>16</v>
       </c>
@@ -1002,8 +1053,11 @@
       <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <v>17</v>
       </c>
@@ -1022,8 +1076,11 @@
       <c r="G15" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <v>18</v>
       </c>
@@ -1041,6 +1098,9 @@
       </c>
       <c r="G16" s="5" t="s">
         <v>38</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1060,7 +1120,10 @@
         <v>15</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -1082,6 +1145,9 @@
       <c r="G18" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="H18" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="19" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
@@ -1102,6 +1168,9 @@
       <c r="G19" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="H19" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
@@ -1122,6 +1191,9 @@
       <c r="G20" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="H20" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
@@ -1142,6 +1214,9 @@
       <c r="G21" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="H21" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
@@ -1162,6 +1237,9 @@
       <c r="G22" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="H22" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="23" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
@@ -1182,15 +1260,84 @@
       <c r="G23" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E24" s="22">
-        <f>SUM(E3:E23)</f>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H27" s="7"/>
+      <c r="H23" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="3">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="5">
+        <v>5</v>
+      </c>
+      <c r="E24" s="6">
+        <v>2</v>
+      </c>
+      <c r="F24" s="4">
+        <v>22</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
+        <v>23</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="5">
+        <v>5</v>
+      </c>
+      <c r="E25" s="6">
+        <v>2</v>
+      </c>
+      <c r="F25" s="4">
+        <v>23</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>24</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="6">
+        <v>4</v>
+      </c>
+      <c r="F26" s="4">
+        <v>24</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="21">
+        <f>SUM(E3:E24)</f>
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="B2:G2">
@@ -1198,7 +1345,7 @@
       <sortCondition ref="F2"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="D3:D23">
+  <conditionalFormatting sqref="D3:D26">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0.5"/>
@@ -1210,10 +1357,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F24">
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F27">
       <formula1>1</formula1>
       <formula2>22</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F26">
+      <formula1>1</formula1>
+      <formula2>24</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1225,7 +1376,7 @@
           <x14:formula1>
             <xm:f>Statuts!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G23</xm:sqref>
+          <xm:sqref>G3:H26</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1253,26 +1404,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B9&amp;" - "&amp;Story!C9</f>
         <v>8 - En tant qu’utilisateur, je veux afficher les arrêts à proximité, sur une carte</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1280,16 +1431,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>8</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>6</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1297,17 +1448,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1315,7 +1466,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>8</v>
       </c>
@@ -1360,26 +1511,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B10&amp;" - "&amp;Story!C10</f>
         <v>12 - En tant qu’utilisateur, je veux afficher les propositions d’itinéraire</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1387,16 +1538,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1404,17 +1555,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1422,7 +1573,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>4</v>
       </c>
@@ -1467,26 +1618,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B11&amp;" - "&amp;Story!C11</f>
         <v>13 - En tant qu’utilisateur, je veux afficher mon itinéraire sur une carte</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1494,13 +1645,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>3</v>
       </c>
       <c r="E4" s="6">
@@ -1511,14 +1662,14 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
       <c r="E5" s="6">
@@ -1529,14 +1680,14 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <f>B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
       <c r="E6" s="6">
@@ -1547,7 +1698,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <f>SUM(E4:E6)</f>
         <v>8</v>
       </c>
@@ -1591,26 +1742,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B12&amp;" - "&amp;Story!C12</f>
         <v>14 - En tant qu’utilisateur, je veux afficher le trajet des lignes sélectionnées sur une carte</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1618,16 +1769,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1635,17 +1786,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1653,7 +1804,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>2</v>
       </c>
@@ -1698,26 +1849,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B13&amp;" - "&amp;Story!C13</f>
         <v>15 - En tant qu’utilisateur, je veux afficher le plan Noctambus en format PDF</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1725,16 +1876,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
-        <v>2</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1742,17 +1893,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1760,7 +1911,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>2</v>
       </c>
@@ -1804,26 +1955,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B14&amp;" - "&amp;Story!C14</f>
         <v>16 - En tant qu’utilisateur, je veux afficher le plan des zones tarifaire en format PDF</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1831,16 +1982,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>13</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>20</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1848,17 +1999,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>5</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1866,7 +2017,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>24</v>
       </c>
@@ -1910,26 +2061,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B15&amp;" - "&amp;Story!C15</f>
         <v>17 - En tant qu’utilisateur, je veux afficher le plan urbain en format PDF</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -1937,16 +2088,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>5</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>6</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -1954,17 +2105,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="18">
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -1972,7 +2123,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>8</v>
       </c>
@@ -2016,26 +2167,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B16&amp;" - "&amp;Story!C16</f>
         <v>18 - En tant qu’utilisateur, je veux afficher le plan périurbain en format PDF</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2043,16 +2194,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>13</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2060,17 +2211,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2078,7 +2229,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>12</v>
       </c>
@@ -2122,26 +2273,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B17&amp;" - "&amp;Story!C17</f>
         <v>9 - En tant qu’utilisateur, je veux acheter un ticket par SMS</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2149,16 +2300,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>5</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2166,17 +2317,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.5</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>1</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2184,7 +2335,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>4</v>
       </c>
@@ -2228,26 +2379,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B18&amp;" - "&amp;Story!C18</f>
         <v>10 - En tant qu’utilisateur, je veux avoir les conditions de vente des tickets</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2255,16 +2406,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.5</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <v>0.5</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2272,17 +2423,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.5</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>0.5</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2290,7 +2441,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>1</v>
       </c>
@@ -2332,52 +2483,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="23">
+      <c r="B2" s="22">
         <v>0.5</v>
       </c>
-      <c r="C2" s="23">
-        <v>1</v>
-      </c>
-      <c r="D2" s="23">
+      <c r="C2" s="22">
+        <v>1</v>
+      </c>
+      <c r="D2" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="24">
+      <c r="B3" s="23">
         <v>3</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="23">
         <v>5</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="23">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>13</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <v>21</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E5" s="23"/>
+      <c r="E5" s="22"/>
       <c r="F5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="24"/>
+      <c r="E6" s="23"/>
       <c r="F6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="25"/>
+      <c r="E7" s="24"/>
       <c r="F7" t="s">
         <v>33</v>
       </c>
@@ -2407,26 +2558,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B19&amp;" - "&amp;Story!C19</f>
         <v>3 - En tant qu’utilisateur, je veux rechercher un arrêt vocalement</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2434,16 +2585,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>0.5</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <v>0.5</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2451,17 +2602,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.5</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>0.5</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2469,7 +2620,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>1</v>
       </c>
@@ -2513,26 +2664,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B20&amp;" - "&amp;Story!C20</f>
         <v>20 - En tant qu’utilisateur, je veux afficher les informations de contact</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2540,16 +2691,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0.5</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <v>0.5</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2557,17 +2708,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>0.5</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>0.5</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2575,7 +2726,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>1</v>
       </c>
@@ -2619,26 +2770,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B21&amp;" - "&amp;Story!C21</f>
         <v>6 - En tant qu’utilisateur, je veux afficher le thermomètre du bus</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2646,16 +2797,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2663,17 +2814,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
         <v>0.5</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2681,7 +2832,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>1.5</v>
       </c>
@@ -2725,26 +2876,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B22&amp;" - "&amp;Story!C22</f>
         <v>21 - En tant qu’utilisateur, je veux afficher les conditions de transport</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2752,16 +2903,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2769,17 +2920,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
         <v>0.5</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2787,7 +2938,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>1.5</v>
       </c>
@@ -2831,26 +2982,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B23&amp;" - "&amp;Story!C23</f>
         <v>19 - En tant qu’utilisateur, je veux afficher les mentions légales</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -2858,16 +3009,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="18">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17">
         <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -2875,17 +3026,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="D5" s="12">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
         <v>0.5</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -2893,7 +3044,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>1.5</v>
       </c>
@@ -2976,26 +3127,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B3&amp;" - "&amp;Story!C3</f>
         <v>1 - En tant qu’utilisateur, je veux afficher la liste des arrêts</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
-    </row>
-    <row r="3" spans="2:6" s="16" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="2:6" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3003,13 +3154,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>2</v>
       </c>
       <c r="E4" s="6">
@@ -3020,14 +3171,14 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
       <c r="E5" s="6">
@@ -3038,14 +3189,14 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <f>B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
       <c r="E6" s="6">
@@ -3056,7 +3207,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <f>SUM(E4:E6)</f>
         <v>8</v>
       </c>
@@ -3101,26 +3252,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B4&amp;" - "&amp;Story!C4</f>
         <v>2 - En tant qu’utilisateur, je veux rechercher un arrêt par nom</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3128,13 +3279,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
       <c r="E4" s="6">
@@ -3145,14 +3296,14 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>1</v>
       </c>
       <c r="E5" s="6">
@@ -3163,7 +3314,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>4</v>
       </c>
@@ -3208,26 +3359,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B5&amp;" - "&amp;Story!C5</f>
         <v>4 - En tant qu’utilisateur, je veux afficher les prochains départs de l’arrêt</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3235,13 +3386,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="12">
         <v>3</v>
       </c>
       <c r="E4" s="6">
@@ -3252,14 +3403,14 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>2</v>
       </c>
       <c r="E5" s="6">
@@ -3270,7 +3421,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>6</v>
       </c>
@@ -3315,26 +3466,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B6&amp;" - "&amp;Story!C6</f>
         <v>11 - En tant qu’utilisateur, je veux saisir mon itinéraire</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3342,13 +3493,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
       <c r="E4" s="6">
@@ -3359,14 +3510,14 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
       <c r="E5" s="6">
@@ -3377,14 +3528,14 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <f>B5+1</f>
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>2</v>
       </c>
       <c r="E6" s="6">
@@ -3395,7 +3546,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <f>SUM(E4:E6)</f>
         <v>12</v>
       </c>
@@ -3441,26 +3592,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B7&amp;" - "&amp;Story!C7</f>
         <v>5 - En tant qu’utilisateur, je veux afficher l’arrêt sélectionné sur une carte</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3468,13 +3619,13 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="10">
         <v>8</v>
       </c>
       <c r="E4" s="6">
@@ -3485,14 +3636,14 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>2</v>
       </c>
       <c r="E5" s="6">
@@ -3503,7 +3654,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>8</v>
       </c>
@@ -3547,26 +3698,26 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>Story!B8&amp;" - "&amp;Story!C8</f>
         <v>7 - En tant qu’utilisateur, je veux afficher la liste des arrêts à proximité</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -3574,16 +3725,16 @@
       </c>
     </row>
     <row r="4" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>13</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="17">
         <v>10</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -3591,17 +3742,17 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+1</f>
         <v>2</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="12">
         <v>3</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="18">
         <v>2</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -3609,7 +3760,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <f>SUM(E4:E5)</f>
         <v>12</v>
       </c>

</xml_diff>